<commit_message>
add cms-kit-management data seeder
</commit_message>
<xml_diff>
--- a/modules/FS.CmsKitManagement/src/FS.CmsKitManagement.Domain.Shared/Files/Blogs.xlsx
+++ b/modules/FS.CmsKitManagement/src/FS.CmsKitManagement.Domain.Shared/Files/Blogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\FS.Works.V4\projects\FS.Abp\modules\FS.CmsKitManagement\src\FS.CmsKitManagement.Domain.Shared\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17841096-728D-4265-936A-FE50B1507586}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6013FC8A-C254-4822-A319-0ACEBB951A2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7110" yWindow="3090" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8715" yWindow="2715" windowWidth="17640" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blogs" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>部落格A</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -721,11 +721,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>http://xin,blog.tw</t>
+    <t>BlogName</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>http://kao,blog.tw</t>
+    <t>http://xin.blog.tw</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://kao.blog.tw</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1067,7 +1071,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1094,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -1107,7 +1111,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1129,10 +1133,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5E5721-6C3E-4492-A306-3DD7A649AC94}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1140,59 +1144,74 @@
     <col min="2" max="2" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[cms-kit-management]angular ui replace cms-kit-modal with fs-tw
</commit_message>
<xml_diff>
--- a/modules/FS.CmsKitManagement/src/FS.CmsKitManagement.Domain.Shared/Files/Blogs.xlsx
+++ b/modules/FS.CmsKitManagement/src/FS.CmsKitManagement.Domain.Shared/Files/Blogs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\FS.Works.V4\projects\FS.Abp\modules\FS.CmsKitManagement\src\FS.CmsKitManagement.Domain.Shared\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\11003\fs.works.v4-1206\projects\FS.Abp\modules\FS.CmsKitManagement\src\FS.CmsKitManagement.Domain.Shared\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6013FC8A-C254-4822-A319-0ACEBB951A2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4E0E52-2395-4229-961D-E0872A403459}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="2715" windowWidth="17640" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-17040" yWindow="-1050" windowWidth="16590" windowHeight="21225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blogs" sheetId="1" r:id="rId1"/>
@@ -1070,17 +1070,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="7" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="2" max="7" width="5.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1106,7 +1106,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1135,84 +1135,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5E5721-6C3E-4492-A306-3DD7A649AC94}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="48.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:3" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
+    <row r="4" spans="1:3" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
+    <row r="5" spans="1:3" ht="16.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>1</v>
-      </c>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="5"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="5"/>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="5"/>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="5"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="5"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
create a cms-author for dataseed
</commit_message>
<xml_diff>
--- a/modules/FS.CmsKitManagement/src/FS.CmsKitManagement.Domain.Shared/Files/Blogs.xlsx
+++ b/modules/FS.CmsKitManagement/src/FS.CmsKitManagement.Domain.Shared/Files/Blogs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\FS.Works.V4\projects\FS.Abp\modules\FS.CmsKitManagement\src\FS.CmsKitManagement.Domain.Shared\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0525\FS-TW\modules\FS.CmsKitManagement\src\FS.CmsKitManagement.Domain.Shared\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016A05B2-E4D0-4D94-999C-6007BF940898}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941ABB56-2625-4F38-82C4-B4FCCE76FBC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="2715" windowWidth="17640" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blogs" sheetId="1" r:id="rId1"/>
-    <sheet name="BlogPosts" sheetId="2" r:id="rId2"/>
+    <sheet name="Author" sheetId="3" r:id="rId1"/>
+    <sheet name="Blogs" sheetId="1" r:id="rId2"/>
+    <sheet name="BlogPosts" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>部落格A</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -746,6 +747,20 @@
   </si>
   <si>
     <t>http://xin.blog.tw/B1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>cms_author@domain.com</t>
+  </si>
+  <si>
+    <t>AuthorName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>cms_author</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1083,6 +1098,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC56972-E7CD-4982-879E-0B43875CBB34}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -1090,13 +1142,13 @@
       <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="7" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.90625" customWidth="1"/>
+    <col min="2" max="7" width="5.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1109,7 +1161,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1174,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1147,112 +1199,128 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B5E5721-6C3E-4492-A306-3DD7A649AC94}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="16.2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{87F8335D-26EC-4801-8928-7C400A52120B}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{F708A2CA-BDF9-4241-867B-74D2A7748CDF}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{BC8E6208-7B4F-462D-986A-1389CA212913}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{27552290-FB21-4D19-991A-8A5FDACA289C}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{87F8335D-26EC-4801-8928-7C400A52120B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{F708A2CA-BDF9-4241-867B-74D2A7748CDF}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{BC8E6208-7B4F-462D-986A-1389CA212913}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{27552290-FB21-4D19-991A-8A5FDACA289C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>